<commit_message>
Update quotes_data.xlsx with new data entries and adjustments for improved accuracy and relevance.
</commit_message>
<xml_diff>
--- a/backend/quotes_data.xlsx
+++ b/backend/quotes_data.xlsx
@@ -715,7 +715,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1377,6 +1377,62 @@
       <c r="N16" t="inlineStr">
         <is>
           <t>2025-09-17T13:01:30.580146</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>faxina</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>47.4</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>unidade</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>2025-09-18T21:24:11.049955</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>2025-09-18T21:24:11.049955</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>eletricista</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>47.4</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>unidade</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>2025-09-18T21:27:57.779088</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>2025-09-18T21:27:57.779088</t>
         </is>
       </c>
     </row>
@@ -1391,7 +1447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1895,6 +1951,88 @@
       <c r="S10" t="inlineStr">
         <is>
           <t>2025-09-17T13:01:31.075613</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>11</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ORC202509009</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Orçamento - faxina</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>limpeza</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>47.4</v>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>2025-09-18T21:24:11.937131</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>2025-09-18T21:24:11.937131</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>12</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ORC202509010</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Orçamento - eletricista</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>manutencao</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+      <c r="M12" t="n">
+        <v>47.4</v>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>2025-09-18T21:27:58.411126</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>2025-09-18T21:27:58.411126</t>
         </is>
       </c>
     </row>
@@ -1909,7 +2047,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2425,6 +2563,88 @@
       <c r="O11" t="inlineStr">
         <is>
           <t>2025-09-17T13:01:31.075613</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>13</v>
+      </c>
+      <c r="B12" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" t="n">
+        <v>16</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>47.4</v>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="n">
+        <v>47.4</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>faxina</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>unidade</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>2025-09-18T21:24:11.937131</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>14</v>
+      </c>
+      <c r="B13" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" t="n">
+        <v>17</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="n">
+        <v>47.4</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="n">
+        <v>47.4</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>eletricista</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>unidade</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>2025-09-18T21:27:58.411126</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhance MLService to introduce realistic price variations based on market context, updating suggested, minimum, and maximum prices accordingly. Also, update reasoning to reflect market variation considerations. Update quotes_data.xlsx with new data entries for improved accuracy.
</commit_message>
<xml_diff>
--- a/backend/quotes_data.xlsx
+++ b/backend/quotes_data.xlsx
@@ -715,7 +715,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1433,6 +1433,62 @@
       <c r="N18" t="inlineStr">
         <is>
           <t>2025-09-18T21:27:57.779088</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>eletrodomesticos</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>47.4</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>unidade</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>2025-09-25T13:53:26.215170</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>2025-09-25T13:53:26.215170</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>dedetizacao</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>129.94</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>unidade</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>2025-09-25T13:58:09.352426</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>2025-09-25T13:58:09.352426</t>
         </is>
       </c>
     </row>
@@ -1447,7 +1503,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2033,6 +2089,88 @@
       <c r="S12" t="inlineStr">
         <is>
           <t>2025-09-18T21:27:58.411126</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>13</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ORC202509011</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Orçamento - eletrodomesticos</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>instalacoes</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+      <c r="M13" t="n">
+        <v>47.4</v>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>2025-09-25T13:53:26.691730</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>2025-09-25T13:53:26.691730</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>14</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ORC202509012</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Orçamento - dedetizacao</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>limpeza</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+      <c r="M14" t="n">
+        <v>129.94</v>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>2025-09-25T13:58:10.103277</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>2025-09-25T13:58:10.103277</t>
         </is>
       </c>
     </row>
@@ -2047,7 +2185,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2645,6 +2783,88 @@
       <c r="O13" t="inlineStr">
         <is>
           <t>2025-09-18T21:27:58.411126</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>15</v>
+      </c>
+      <c r="B14" t="n">
+        <v>13</v>
+      </c>
+      <c r="C14" t="n">
+        <v>18</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" t="n">
+        <v>47.4</v>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="n">
+        <v>47.4</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>eletrodomesticos</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>unidade</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>2025-09-25T13:53:26.691730</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>16</v>
+      </c>
+      <c r="B15" t="n">
+        <v>14</v>
+      </c>
+      <c r="C15" t="n">
+        <v>19</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" t="n">
+        <v>129.94</v>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="n">
+        <v>129.94</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>dedetizacao</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>unidade</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>2025-09-25T13:58:10.103277</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor MLService to include methods for generating professional titles and descriptions based on service categories. Update ML prediction response structure in frontend to display new fields: professional title and technical specifications. Modify UI labels for clarity and consistency.
</commit_message>
<xml_diff>
--- a/backend/quotes_data.xlsx
+++ b/backend/quotes_data.xlsx
@@ -715,7 +715,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1489,6 +1489,34 @@
       <c r="N20" t="inlineStr">
         <is>
           <t>2025-09-25T13:58:09.352426</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>mudancas</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>52.13</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>unidade</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>2025-09-25T14:04:10.329003</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>2025-09-25T14:04:10.329003</t>
         </is>
       </c>
     </row>
@@ -1503,7 +1531,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2171,6 +2199,47 @@
       <c r="S14" t="inlineStr">
         <is>
           <t>2025-09-25T13:58:10.103277</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>15</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ORC202509013</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Orçamento - mudancas</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>gerais</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+      <c r="M15" t="n">
+        <v>52.13</v>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>2025-09-25T14:04:10.698587</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>2025-09-25T14:04:10.698587</t>
         </is>
       </c>
     </row>
@@ -2185,7 +2254,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2865,6 +2934,47 @@
       <c r="O15" t="inlineStr">
         <is>
           <t>2025-09-25T13:58:10.103277</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>17</v>
+      </c>
+      <c r="B16" t="n">
+        <v>15</v>
+      </c>
+      <c r="C16" t="n">
+        <v>20</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="n">
+        <v>52.13</v>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="n">
+        <v>52.13</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>mudancas</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>unidade</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>2025-09-25T14:04:10.698587</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor frontend screens to implement a dark theme and enhance UI consistency. Update color schemes, remove unused navigation methods, and replace logo widget across multiple screens. Adjust footer menu and input styles for improved aesthetics and usability.
</commit_message>
<xml_diff>
--- a/backend/quotes_data.xlsx
+++ b/backend/quotes_data.xlsx
@@ -21,9 +21,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -716,7 +715,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1546,6 +1545,90 @@
       <c r="N22" t="inlineStr">
         <is>
           <t>2025-09-25T14:05:34.547850</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>encanador</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>97.33</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>unidade</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>2025-10-01T11:10:51.671790</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>2025-10-01T11:10:51.671790</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>eletricista</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>42.65</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>unidade</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>2025-10-01T11:13:01.121166</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>2025-10-01T11:13:01.121166</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>pintor</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>251.14</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>unidade</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>2025-10-01T11:41:51.503802</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>2025-10-01T11:41:51.503802</t>
         </is>
       </c>
     </row>
@@ -1560,7 +1643,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1728,7 +1811,6 @@
       <c r="P2" t="n">
         <v>0</v>
       </c>
-      <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr">
         <is>
           <t>2025-09-12T12:12:00.892057</t>
@@ -1762,24 +1844,14 @@
           <t>Serviço residencial encanador de alta qualidade e confiabilidade</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
           <t>approved</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
       <c r="M3" t="n">
         <v>50</v>
       </c>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr">
         <is>
           <t>2025-09-12T19:00:07.990321</t>
@@ -1813,24 +1885,14 @@
           <t>Serviço residencial gesseiro de alta qualidade e confiabilidade</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
           <t>pendente</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
       <c r="M4" t="n">
         <v>50</v>
       </c>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr">
         <is>
           <t>2025-09-12T19:03:47.500109</t>
@@ -1864,24 +1926,14 @@
           <t>Pintor profissional para sua residência. Serviço de pintura interna e externa, utilizando materiais de alta qualidade. Renove seu ambiente com cores vibrantes e durabilidade garantida. Entre em contato para um orçamento personalizado.</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
           <t>pendente</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
       <c r="M5" t="n">
         <v>500</v>
       </c>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr">
         <is>
           <t>2025-09-12T19:06:32.447976</t>
@@ -1915,24 +1967,14 @@
           <t>Serviço de serralheria residencial com fabricação e instalação de portões, grades, corrimãos e estruturas metálicas. Qualidade, segurança e durabilidade garantidas. Entre em contato para um orçamento personalizado.</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>pendente</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
         <v>150</v>
       </c>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr">
         <is>
           <t>2025-09-12T19:13:43.961201</t>
@@ -1966,24 +2008,14 @@
           <t>Serviço de jardinagem residencial profissional, incluindo corte de grama, poda de árvores e plantas, adubação e controle de pragas. Transforme seu jardim em um ambiente mais agradável e bonito. Solicite seu orçamento agora.</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
           <t>pendente</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
       <c r="M7" t="n">
         <v>250</v>
       </c>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr">
         <is>
           <t>2025-09-12T19:21:54.788628</t>
@@ -2017,24 +2049,14 @@
           <t>Serviço de jardinagem profissional para manutenção de jardins residenciais. Corte de grama, poda de árvores e plantas, controle de ervas daninhas e adubação. Transforme seu jardim em um ambiente agradável e bem cuidado.</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
           <t>pendente</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
       <c r="M8" t="n">
         <v>150</v>
       </c>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr">
         <is>
           <t>2025-09-15T21:23:16.578461</t>
@@ -2068,24 +2090,14 @@
           <t>manutencao</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
           <t>pendente</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
       <c r="M9" t="n">
         <v>100.4</v>
       </c>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr">
         <is>
           <t>2025-09-17T12:57:36.612668</t>
@@ -2119,24 +2131,14 @@
           <t>limpeza</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
           <t>pendente</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
       <c r="M10" t="n">
         <v>47.4</v>
       </c>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
       <c r="R10" t="inlineStr">
         <is>
           <t>2025-09-17T13:01:31.075613</t>
@@ -2170,24 +2172,14 @@
           <t>limpeza</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
           <t>pendente</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
       <c r="M11" t="n">
         <v>47.4</v>
       </c>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
       <c r="R11" t="inlineStr">
         <is>
           <t>2025-09-18T21:24:11.937131</t>
@@ -2221,24 +2213,14 @@
           <t>manutencao</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
           <t>pendente</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
       <c r="M12" t="n">
         <v>47.4</v>
       </c>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
       <c r="R12" t="inlineStr">
         <is>
           <t>2025-09-18T21:27:58.411126</t>
@@ -2272,24 +2254,14 @@
           <t>instalacoes</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
           <t>pendente</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
       <c r="M13" t="n">
         <v>47.4</v>
       </c>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
       <c r="R13" t="inlineStr">
         <is>
           <t>2025-09-25T13:53:26.691730</t>
@@ -2323,24 +2295,14 @@
           <t>limpeza</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
           <t>pendente</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
       <c r="M14" t="n">
         <v>129.94</v>
       </c>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr">
         <is>
           <t>2025-09-25T13:58:10.103277</t>
@@ -2374,24 +2336,14 @@
           <t>gerais</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
           <t>pendente</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
       <c r="M15" t="n">
         <v>52.13</v>
       </c>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr"/>
       <c r="R15" t="inlineStr">
         <is>
           <t>2025-09-25T14:04:10.698587</t>
@@ -2425,24 +2377,14 @@
           <t>instalacoes</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
         <is>
           <t>pendente</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
       <c r="M16" t="n">
         <v>132.3</v>
       </c>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr">
         <is>
           <t>2025-09-25T14:05:34.859157</t>
@@ -2451,6 +2393,129 @@
       <c r="S16" t="inlineStr">
         <is>
           <t>2025-09-25T14:05:34.859157</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>17</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ORC202510001</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Orçamento - encanador</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>manutencao</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+      <c r="M17" t="n">
+        <v>97.33</v>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>2025-10-01T11:10:52.195030</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>2025-10-01T11:10:52.195030</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>18</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ORC202510002</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Orçamento - eletricista</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>manutencao</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+      <c r="M18" t="n">
+        <v>42.65</v>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>2025-10-01T11:13:01.833293</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>2025-10-01T11:13:01.833293</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>19</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ORC202510003</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Orçamento - pintor</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>manutencao</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+      <c r="M19" t="n">
+        <v>251.14</v>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>2025-10-01T11:41:52.131080</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>2025-10-01T11:41:52.131080</t>
         </is>
       </c>
     </row>
@@ -2465,7 +2530,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2600,6 +2665,8 @@
       <c r="M2" t="n">
         <v>0</v>
       </c>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -2651,6 +2718,8 @@
       <c r="M3" t="n">
         <v>0</v>
       </c>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -2668,6 +2737,7 @@
       <c r="E4" t="n">
         <v>50</v>
       </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="n">
         <v>50</v>
       </c>
@@ -2676,11 +2746,16 @@
           <t>encanador</t>
         </is>
       </c>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
           <t>unidade</t>
         </is>
       </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr">
         <is>
           <t>2025-09-12T19:00:07.990321</t>
@@ -2703,6 +2778,7 @@
       <c r="E5" t="n">
         <v>50</v>
       </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="n">
         <v>50</v>
       </c>
@@ -2711,11 +2787,16 @@
           <t>gesseiro</t>
         </is>
       </c>
+      <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
           <t>unidade</t>
         </is>
       </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr">
         <is>
           <t>2025-09-12T19:03:47.500109</t>
@@ -2738,6 +2819,7 @@
       <c r="E6" t="n">
         <v>500</v>
       </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="n">
         <v>500</v>
       </c>
@@ -2746,11 +2828,16 @@
           <t>pintor</t>
         </is>
       </c>
+      <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr">
         <is>
           <t>unidade</t>
         </is>
       </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr">
         <is>
           <t>2025-09-12T19:06:32.447976</t>
@@ -2773,6 +2860,7 @@
       <c r="E7" t="n">
         <v>150</v>
       </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
         <v>150</v>
       </c>
@@ -2781,11 +2869,16 @@
           <t>serralheria</t>
         </is>
       </c>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
           <t>unidade</t>
         </is>
       </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr">
         <is>
           <t>2025-09-12T19:13:43.961201</t>
@@ -2808,6 +2901,7 @@
       <c r="E8" t="n">
         <v>250</v>
       </c>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="n">
         <v>250</v>
       </c>
@@ -2816,11 +2910,16 @@
           <t>jardinagem</t>
         </is>
       </c>
+      <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
           <t>unidade</t>
         </is>
       </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr">
         <is>
           <t>2025-09-12T19:21:54.788628</t>
@@ -2843,6 +2942,7 @@
       <c r="E9" t="n">
         <v>150</v>
       </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
         <v>150</v>
       </c>
@@ -2851,11 +2951,16 @@
           <t>jardinagem</t>
         </is>
       </c>
+      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
         <is>
           <t>unidade</t>
         </is>
       </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr">
         <is>
           <t>2025-09-15T21:23:16.578461</t>
@@ -2878,6 +2983,7 @@
       <c r="E10" t="n">
         <v>100.4</v>
       </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="n">
         <v>100.4</v>
       </c>
@@ -2886,11 +2992,16 @@
           <t>encanador</t>
         </is>
       </c>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr">
         <is>
           <t>unidade</t>
         </is>
       </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr">
         <is>
           <t>2025-09-17T12:57:36.612668</t>
@@ -2913,6 +3024,7 @@
       <c r="E11" t="n">
         <v>47.4</v>
       </c>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="n">
         <v>47.4</v>
       </c>
@@ -2921,11 +3033,16 @@
           <t>faxina</t>
         </is>
       </c>
+      <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr">
         <is>
           <t>unidade</t>
         </is>
       </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr">
         <is>
           <t>2025-09-17T13:01:31.075613</t>
@@ -2948,6 +3065,7 @@
       <c r="E12" t="n">
         <v>47.4</v>
       </c>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
         <v>47.4</v>
       </c>
@@ -2956,11 +3074,16 @@
           <t>faxina</t>
         </is>
       </c>
+      <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr">
         <is>
           <t>unidade</t>
         </is>
       </c>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr">
         <is>
           <t>2025-09-18T21:24:11.937131</t>
@@ -2983,6 +3106,7 @@
       <c r="E13" t="n">
         <v>47.4</v>
       </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
         <v>47.4</v>
       </c>
@@ -2991,11 +3115,16 @@
           <t>eletricista</t>
         </is>
       </c>
+      <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
           <t>unidade</t>
         </is>
       </c>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr">
         <is>
           <t>2025-09-18T21:27:58.411126</t>
@@ -3018,6 +3147,7 @@
       <c r="E14" t="n">
         <v>47.4</v>
       </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
         <v>47.4</v>
       </c>
@@ -3026,11 +3156,16 @@
           <t>eletrodomesticos</t>
         </is>
       </c>
+      <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr">
         <is>
           <t>unidade</t>
         </is>
       </c>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr">
         <is>
           <t>2025-09-25T13:53:26.691730</t>
@@ -3053,6 +3188,7 @@
       <c r="E15" t="n">
         <v>129.94</v>
       </c>
+      <c r="F15" t="inlineStr"/>
       <c r="G15" t="n">
         <v>129.94</v>
       </c>
@@ -3061,11 +3197,16 @@
           <t>dedetizacao</t>
         </is>
       </c>
+      <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
           <t>unidade</t>
         </is>
       </c>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr">
         <is>
           <t>2025-09-25T13:58:10.103277</t>
@@ -3088,6 +3229,7 @@
       <c r="E16" t="n">
         <v>52.13</v>
       </c>
+      <c r="F16" t="inlineStr"/>
       <c r="G16" t="n">
         <v>52.13</v>
       </c>
@@ -3096,11 +3238,16 @@
           <t>mudancas</t>
         </is>
       </c>
+      <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr">
         <is>
           <t>unidade</t>
         </is>
       </c>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr">
         <is>
           <t>2025-09-25T14:04:10.698587</t>
@@ -3123,6 +3270,7 @@
       <c r="E17" t="n">
         <v>132.3</v>
       </c>
+      <c r="F17" t="inlineStr"/>
       <c r="G17" t="n">
         <v>132.3</v>
       </c>
@@ -3131,14 +3279,142 @@
           <t>montagem</t>
         </is>
       </c>
+      <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr">
         <is>
           <t>unidade</t>
         </is>
       </c>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr">
         <is>
           <t>2025-09-25T14:05:34.859157</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>19</v>
+      </c>
+      <c r="B18" t="n">
+        <v>17</v>
+      </c>
+      <c r="C18" t="n">
+        <v>22</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" t="n">
+        <v>97.33</v>
+      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="n">
+        <v>97.33</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>encanador</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>unidade</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>2025-10-01T11:10:52.195030</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>20</v>
+      </c>
+      <c r="B19" t="n">
+        <v>18</v>
+      </c>
+      <c r="C19" t="n">
+        <v>23</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="n">
+        <v>42.65</v>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="n">
+        <v>42.65</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>eletricista</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>unidade</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>2025-10-01T11:13:01.833293</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>21</v>
+      </c>
+      <c r="B20" t="n">
+        <v>19</v>
+      </c>
+      <c r="C20" t="n">
+        <v>24</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" t="n">
+        <v>251.14</v>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="n">
+        <v>251.14</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>pintor</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>unidade</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>2025-10-01T11:41:52.131080</t>
         </is>
       </c>
     </row>

</xml_diff>